<commit_message>
added toggle to change calc settings
added calc step and max income inputs to app
misc edits to fix poorly named functions etc
</commit_message>
<xml_diff>
--- a/taxes.xlsx
+++ b/taxes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joelfindlay/Documents/GitHub/taxes_and_transfers/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD740DDF-08ED-0747-875A-F262F2A9F270}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2CCF011-D57F-C740-AA85-BF13BDF07FAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="27780" windowHeight="17500" xr2:uid="{DD1CEF2E-34E4-5F45-A5C0-3EEDD9DFA19E}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="27780" windowHeight="17500" activeTab="1" xr2:uid="{DD1CEF2E-34E4-5F45-A5C0-3EEDD9DFA19E}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="7" r:id="rId1"/>
@@ -1364,7 +1364,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{498AA68C-CFF6-074F-9A1F-DD54B9C8ADA9}">
   <dimension ref="A1:J43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
@@ -1808,8 +1808,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AC324EE-D799-1E44-ABC6-DF64E0EB172D}">
   <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2512,7 +2512,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADD11409-4DF5-E04A-9CAB-99924B334ABB}">
   <dimension ref="A1:G40"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0">
+    <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
@@ -3569,7 +3569,7 @@
   <dimension ref="A1:P11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>